<commit_message>
Update material with new mongooses
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="377">
   <si>
     <t>type_id</t>
   </si>
@@ -6262,7 +6262,9 @@
       <c r="D159" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E159" s="1"/>
+      <c r="E159" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1">
@@ -6319,13 +6321,13 @@
       <c r="C161" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F161" s="1"/>
+      <c r="D161" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F161" s="4"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1">
         <v>4.0</v>
@@ -6350,13 +6352,11 @@
       <c r="C162" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G162" s="1"/>
       <c r="H162" s="1">
         <v>5.0</v>
@@ -6381,8 +6381,12 @@
       <c r="C163" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
+      <c r="D163" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1">

</xml_diff>

<commit_message>
Update material for beavers
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="378">
   <si>
     <t>type_id</t>
   </si>
@@ -564,16 +564,19 @@
     <t>Next time you have gained a new 🃏 from the market, take any 1 🃏 from your discard.</t>
   </si>
   <si>
+    <t>onMarketCard</t>
+  </si>
+  <si>
+    <t>Beavers</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Next time before you build, take 1 🃏 from the market.</t>
+  </si>
+  <si>
     <t>onClient</t>
-  </si>
-  <si>
-    <t>Beavers</t>
-  </si>
-  <si>
-    <t>Snack</t>
-  </si>
-  <si>
-    <t>Next time before you build, take 1 🃏 from the market.</t>
   </si>
   <si>
     <t>Wind of Change</t>
@@ -3827,7 +3830,7 @@
         <v>18</v>
       </c>
       <c r="F80" s="3"/>
-      <c r="G80" s="1" t="s">
+      <c r="G80" s="4" t="s">
         <v>182</v>
       </c>
       <c r="H80" s="3">
@@ -3859,7 +3862,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H81" s="1">
         <v>2.0</v>
@@ -3879,10 +3882,10 @@
         <v>80.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>18</v>
@@ -3912,10 +3915,10 @@
         <v>81.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>18</v>
@@ -3925,7 +3928,7 @@
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H83" s="1">
         <v>4.0</v>
@@ -3945,10 +3948,10 @@
         <v>82.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>18</v>
@@ -3978,10 +3981,10 @@
         <v>83.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>18</v>
@@ -4011,10 +4014,10 @@
         <v>84.0</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -4027,7 +4030,7 @@
         <v>0.0</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K86" s="10">
         <v>14.0</v>
@@ -4038,10 +4041,10 @@
         <v>85.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4056,7 +4059,7 @@
         <v>3.0</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K87" s="9">
         <v>14.0</v>
@@ -4067,10 +4070,10 @@
         <v>86.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>18</v>
@@ -4087,7 +4090,7 @@
         <v>3.0</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K88" s="9">
         <v>14.0</v>
@@ -4098,10 +4101,10 @@
         <v>87.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>18</v>
@@ -4118,7 +4121,7 @@
         <v>3.0</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K89" s="9">
         <v>14.0</v>
@@ -4129,10 +4132,10 @@
         <v>88.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>18</v>
@@ -4149,7 +4152,7 @@
         <v>1.0</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K90" s="9">
         <v>14.0</v>
@@ -4160,10 +4163,10 @@
         <v>89.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4178,7 +4181,7 @@
         <v>1.0</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K91" s="9">
         <v>14.0</v>
@@ -4189,10 +4192,10 @@
         <v>90.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>18</v>
@@ -4209,7 +4212,7 @@
         <v>0.0</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K92" s="9">
         <v>15.0</v>
@@ -4220,10 +4223,10 @@
         <v>91.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>18</v>
@@ -4240,7 +4243,7 @@
         <v>3.0</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K93" s="9">
         <v>15.0</v>
@@ -4251,10 +4254,10 @@
         <v>92.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>18</v>
@@ -4269,7 +4272,7 @@
         <v>3.0</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K94" s="9">
         <v>15.0</v>
@@ -4280,10 +4283,10 @@
         <v>93.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>18</v>
@@ -4300,7 +4303,7 @@
         <v>3.0</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K95" s="9">
         <v>15.0</v>
@@ -4311,10 +4314,10 @@
         <v>94.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>18</v>
@@ -4331,7 +4334,7 @@
         <v>1.0</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K96" s="9">
         <v>15.0</v>
@@ -4342,10 +4345,10 @@
         <v>95.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4358,7 +4361,7 @@
         <v>1.0</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K97" s="9">
         <v>15.0</v>
@@ -4369,10 +4372,10 @@
         <v>96.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>18</v>
@@ -4389,7 +4392,7 @@
         <v>0.0</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K98" s="9">
         <v>16.0</v>
@@ -4400,10 +4403,10 @@
         <v>97.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4416,7 +4419,7 @@
         <v>3.0</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K99" s="9">
         <v>16.0</v>
@@ -4427,10 +4430,10 @@
         <v>98.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>18</v>
@@ -4447,7 +4450,7 @@
         <v>3.0</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K100" s="9">
         <v>16.0</v>
@@ -4458,10 +4461,10 @@
         <v>99.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>18</v>
@@ -4478,7 +4481,7 @@
         <v>3.0</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K101" s="9">
         <v>16.0</v>
@@ -4489,10 +4492,10 @@
         <v>100.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>18</v>
@@ -4509,7 +4512,7 @@
         <v>1.0</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K102" s="9">
         <v>16.0</v>
@@ -4520,10 +4523,10 @@
         <v>101.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>18</v>
@@ -4540,7 +4543,7 @@
         <v>1.0</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K103" s="9">
         <v>16.0</v>
@@ -4551,10 +4554,10 @@
         <v>102.0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>18</v>
@@ -4571,7 +4574,7 @@
         <v>0.0</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K104" s="9">
         <v>17.0</v>
@@ -4582,10 +4585,10 @@
         <v>103.0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -4600,7 +4603,7 @@
         <v>3.0</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K105" s="9">
         <v>17.0</v>
@@ -4611,10 +4614,10 @@
         <v>104.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>18</v>
@@ -4631,7 +4634,7 @@
         <v>3.0</v>
       </c>
       <c r="J106" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K106" s="9">
         <v>17.0</v>
@@ -4642,10 +4645,10 @@
         <v>105.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>18</v>
@@ -4662,7 +4665,7 @@
         <v>3.0</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K107" s="9">
         <v>17.0</v>
@@ -4673,10 +4676,10 @@
         <v>106.0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>18</v>
@@ -4693,7 +4696,7 @@
         <v>1.0</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K108" s="9">
         <v>17.0</v>
@@ -4704,10 +4707,10 @@
         <v>107.0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>18</v>
@@ -4724,7 +4727,7 @@
         <v>1.0</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K109" s="9">
         <v>17.0</v>
@@ -4735,10 +4738,10 @@
         <v>108.0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -4753,7 +4756,7 @@
         <v>0.0</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K110" s="9">
         <v>18.0</v>
@@ -4764,10 +4767,10 @@
         <v>109.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -4782,7 +4785,7 @@
         <v>3.0</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K111" s="9">
         <v>18.0</v>
@@ -4793,10 +4796,10 @@
         <v>110.0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>18</v>
@@ -4813,7 +4816,7 @@
         <v>3.0</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K112" s="9">
         <v>18.0</v>
@@ -4824,10 +4827,10 @@
         <v>111.0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>18</v>
@@ -4844,7 +4847,7 @@
         <v>3.0</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K113" s="9">
         <v>18.0</v>
@@ -4855,10 +4858,10 @@
         <v>112.0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>18</v>
@@ -4875,7 +4878,7 @@
         <v>1.0</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K114" s="9">
         <v>18.0</v>
@@ -4886,10 +4889,10 @@
         <v>113.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -4904,7 +4907,7 @@
         <v>1.0</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K115" s="9">
         <v>18.0</v>
@@ -4915,10 +4918,10 @@
         <v>114.0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>18</v>
@@ -4937,7 +4940,7 @@
         <v>0.0</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K116" s="9">
         <v>19.0</v>
@@ -4948,10 +4951,10 @@
         <v>115.0</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -4968,7 +4971,7 @@
         <v>3.0</v>
       </c>
       <c r="J117" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K117" s="9">
         <v>19.0</v>
@@ -4979,10 +4982,10 @@
         <v>116.0</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>18</v>
@@ -5001,7 +5004,7 @@
         <v>3.0</v>
       </c>
       <c r="J118" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K118" s="9">
         <v>19.0</v>
@@ -5012,10 +5015,10 @@
         <v>117.0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>18</v>
@@ -5034,7 +5037,7 @@
         <v>3.0</v>
       </c>
       <c r="J119" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K119" s="9">
         <v>19.0</v>
@@ -5045,10 +5048,10 @@
         <v>118.0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>18</v>
@@ -5067,7 +5070,7 @@
         <v>1.0</v>
       </c>
       <c r="J120" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K120" s="9">
         <v>19.0</v>
@@ -5078,10 +5081,10 @@
         <v>119.0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -5096,7 +5099,7 @@
         <v>1.0</v>
       </c>
       <c r="J121" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K121" s="9">
         <v>19.0</v>
@@ -5107,10 +5110,10 @@
         <v>120.0</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>18</v>
@@ -5127,7 +5130,7 @@
         <v>0.0</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K122" s="10">
         <v>20.0</v>
@@ -5138,10 +5141,10 @@
         <v>121.0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>18</v>
@@ -5156,7 +5159,7 @@
         <v>3.0</v>
       </c>
       <c r="J123" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K123" s="9">
         <v>20.0</v>
@@ -5167,10 +5170,10 @@
         <v>122.0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>18</v>
@@ -5187,7 +5190,7 @@
         <v>3.0</v>
       </c>
       <c r="J124" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K124" s="9">
         <v>20.0</v>
@@ -5198,10 +5201,10 @@
         <v>123.0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -5214,7 +5217,7 @@
         <v>3.0</v>
       </c>
       <c r="J125" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K125" s="9">
         <v>20.0</v>
@@ -5225,10 +5228,10 @@
         <v>124.0</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>18</v>
@@ -5245,7 +5248,7 @@
         <v>1.0</v>
       </c>
       <c r="J126" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K126" s="9">
         <v>20.0</v>
@@ -5256,10 +5259,10 @@
         <v>125.0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>18</v>
@@ -5276,7 +5279,7 @@
         <v>1.0</v>
       </c>
       <c r="J127" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K127" s="9">
         <v>20.0</v>
@@ -5287,10 +5290,10 @@
         <v>126.0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>18</v>
@@ -5309,7 +5312,7 @@
         <v>0.0</v>
       </c>
       <c r="J128" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K128" s="9">
         <v>21.0</v>
@@ -5320,10 +5323,10 @@
         <v>127.0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -5338,7 +5341,7 @@
         <v>3.0</v>
       </c>
       <c r="J129" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K129" s="9">
         <v>21.0</v>
@@ -5349,10 +5352,10 @@
         <v>128.0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>18</v>
@@ -5369,7 +5372,7 @@
         <v>3.0</v>
       </c>
       <c r="J130" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K130" s="9">
         <v>21.0</v>
@@ -5380,10 +5383,10 @@
         <v>129.0</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>18</v>
@@ -5400,7 +5403,7 @@
         <v>3.0</v>
       </c>
       <c r="J131" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K131" s="9">
         <v>21.0</v>
@@ -5411,10 +5414,10 @@
         <v>130.0</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>18</v>
@@ -5431,7 +5434,7 @@
         <v>1.0</v>
       </c>
       <c r="J132" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K132" s="9">
         <v>21.0</v>
@@ -5442,10 +5445,10 @@
         <v>131.0</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>18</v>
@@ -5462,7 +5465,7 @@
         <v>1.0</v>
       </c>
       <c r="J133" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K133" s="9">
         <v>21.0</v>
@@ -5473,10 +5476,10 @@
         <v>132.0</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>18</v>
@@ -5486,7 +5489,7 @@
       </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H134" s="1">
         <v>1.0</v>
@@ -5495,7 +5498,7 @@
         <v>0.0</v>
       </c>
       <c r="J134" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K134" s="9">
         <v>22.0</v>
@@ -5506,10 +5509,10 @@
         <v>133.0</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>18</v>
@@ -5517,7 +5520,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H135" s="1">
         <v>2.0</v>
@@ -5526,7 +5529,7 @@
         <v>3.0</v>
       </c>
       <c r="J135" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K135" s="9">
         <v>22.0</v>
@@ -5537,10 +5540,10 @@
         <v>134.0</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>18</v>
@@ -5550,7 +5553,7 @@
       </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H136" s="1">
         <v>3.0</v>
@@ -5559,7 +5562,7 @@
         <v>3.0</v>
       </c>
       <c r="J136" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K136" s="9">
         <v>22.0</v>
@@ -5570,10 +5573,10 @@
         <v>135.0</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>18</v>
@@ -5583,7 +5586,7 @@
       </c>
       <c r="F137" s="1"/>
       <c r="G137" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H137" s="1">
         <v>4.0</v>
@@ -5592,7 +5595,7 @@
         <v>3.0</v>
       </c>
       <c r="J137" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K137" s="9">
         <v>22.0</v>
@@ -5603,10 +5606,10 @@
         <v>136.0</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>18</v>
@@ -5616,7 +5619,7 @@
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H138" s="1">
         <v>5.0</v>
@@ -5625,7 +5628,7 @@
         <v>1.0</v>
       </c>
       <c r="J138" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K138" s="9">
         <v>22.0</v>
@@ -5636,10 +5639,10 @@
         <v>137.0</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>18</v>
@@ -5649,7 +5652,7 @@
       </c>
       <c r="F139" s="1"/>
       <c r="G139" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H139" s="1">
         <v>5.0</v>
@@ -5658,7 +5661,7 @@
         <v>1.0</v>
       </c>
       <c r="J139" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K139" s="9">
         <v>22.0</v>
@@ -5669,10 +5672,10 @@
         <v>138.0</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>18</v>
@@ -5689,7 +5692,7 @@
         <v>0.0</v>
       </c>
       <c r="J140" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K140" s="9">
         <v>23.0</v>
@@ -5700,10 +5703,10 @@
         <v>139.0</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>18</v>
@@ -5720,7 +5723,7 @@
         <v>3.0</v>
       </c>
       <c r="J141" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K141" s="9">
         <v>23.0</v>
@@ -5731,10 +5734,10 @@
         <v>140.0</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>18</v>
@@ -5751,7 +5754,7 @@
         <v>3.0</v>
       </c>
       <c r="J142" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K142" s="9">
         <v>23.0</v>
@@ -5762,10 +5765,10 @@
         <v>141.0</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>18</v>
@@ -5782,7 +5785,7 @@
         <v>3.0</v>
       </c>
       <c r="J143" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K143" s="9">
         <v>23.0</v>
@@ -5793,10 +5796,10 @@
         <v>142.0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>18</v>
@@ -5813,7 +5816,7 @@
         <v>1.0</v>
       </c>
       <c r="J144" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K144" s="9">
         <v>23.0</v>
@@ -5824,10 +5827,10 @@
         <v>143.0</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>18</v>
@@ -5844,7 +5847,7 @@
         <v>1.0</v>
       </c>
       <c r="J145" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K145" s="9">
         <v>23.0</v>
@@ -5855,10 +5858,10 @@
         <v>144.0</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>18</v>
@@ -5875,7 +5878,7 @@
         <v>0.0</v>
       </c>
       <c r="J146" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K146" s="9">
         <v>24.0</v>
@@ -5886,10 +5889,10 @@
         <v>145.0</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -5904,7 +5907,7 @@
         <v>3.0</v>
       </c>
       <c r="J147" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K147" s="9">
         <v>24.0</v>
@@ -5915,10 +5918,10 @@
         <v>146.0</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>18</v>
@@ -5935,7 +5938,7 @@
         <v>3.0</v>
       </c>
       <c r="J148" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K148" s="9">
         <v>24.0</v>
@@ -5946,10 +5949,10 @@
         <v>147.0</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>18</v>
@@ -5966,7 +5969,7 @@
         <v>3.0</v>
       </c>
       <c r="J149" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K149" s="9">
         <v>24.0</v>
@@ -5977,10 +5980,10 @@
         <v>148.0</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>18</v>
@@ -5997,7 +6000,7 @@
         <v>1.0</v>
       </c>
       <c r="J150" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K150" s="9">
         <v>24.0</v>
@@ -6008,10 +6011,10 @@
         <v>149.0</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>18</v>
@@ -6028,7 +6031,7 @@
         <v>1.0</v>
       </c>
       <c r="J151" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K151" s="9">
         <v>24.0</v>
@@ -6039,10 +6042,10 @@
         <v>150.0</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>18</v>
@@ -6059,7 +6062,7 @@
         <v>0.0</v>
       </c>
       <c r="J152" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K152" s="9">
         <v>25.0</v>
@@ -6070,10 +6073,10 @@
         <v>151.0</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>18</v>
@@ -6090,7 +6093,7 @@
         <v>3.0</v>
       </c>
       <c r="J153" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K153" s="9">
         <v>25.0</v>
@@ -6101,10 +6104,10 @@
         <v>152.0</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>18</v>
@@ -6121,7 +6124,7 @@
         <v>3.0</v>
       </c>
       <c r="J154" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K154" s="9">
         <v>25.0</v>
@@ -6132,10 +6135,10 @@
         <v>153.0</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>18</v>
@@ -6152,7 +6155,7 @@
         <v>3.0</v>
       </c>
       <c r="J155" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K155" s="9">
         <v>25.0</v>
@@ -6163,10 +6166,10 @@
         <v>154.0</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>18</v>
@@ -6183,7 +6186,7 @@
         <v>1.0</v>
       </c>
       <c r="J156" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K156" s="9">
         <v>25.0</v>
@@ -6194,10 +6197,10 @@
         <v>155.0</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>18</v>
@@ -6214,7 +6217,7 @@
         <v>1.0</v>
       </c>
       <c r="J157" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K157" s="9">
         <v>25.0</v>
@@ -6225,10 +6228,10 @@
         <v>156.0</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
@@ -6243,7 +6246,7 @@
         <v>0.0</v>
       </c>
       <c r="J158" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K158" s="9">
         <v>26.0</v>
@@ -6254,10 +6257,10 @@
         <v>157.0</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>18</v>
@@ -6274,7 +6277,7 @@
         <v>3.0</v>
       </c>
       <c r="J159" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K159" s="9">
         <v>26.0</v>
@@ -6285,10 +6288,10 @@
         <v>158.0</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>18</v>
@@ -6305,7 +6308,7 @@
         <v>3.0</v>
       </c>
       <c r="J160" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K160" s="9">
         <v>26.0</v>
@@ -6316,10 +6319,10 @@
         <v>159.0</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>18</v>
@@ -6336,7 +6339,7 @@
         <v>3.0</v>
       </c>
       <c r="J161" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K161" s="9">
         <v>26.0</v>
@@ -6347,10 +6350,10 @@
         <v>160.0</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -6365,7 +6368,7 @@
         <v>1.0</v>
       </c>
       <c r="J162" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K162" s="9">
         <v>26.0</v>
@@ -6376,10 +6379,10 @@
         <v>161.0</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>18</v>
@@ -6394,7 +6397,7 @@
         <v>1.0</v>
       </c>
       <c r="J163" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K163" s="9">
         <v>26.0</v>
@@ -6405,10 +6408,10 @@
         <v>162.0</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>18</v>
@@ -6425,7 +6428,7 @@
         <v>0.0</v>
       </c>
       <c r="J164" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K164" s="9">
         <v>27.0</v>
@@ -6436,10 +6439,10 @@
         <v>163.0</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>18</v>
@@ -6456,7 +6459,7 @@
         <v>3.0</v>
       </c>
       <c r="J165" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K165" s="9">
         <v>27.0</v>
@@ -6467,10 +6470,10 @@
         <v>164.0</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>18</v>
@@ -6487,7 +6490,7 @@
         <v>3.0</v>
       </c>
       <c r="J166" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K166" s="9">
         <v>27.0</v>
@@ -6498,10 +6501,10 @@
         <v>165.0</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>18</v>
@@ -6518,7 +6521,7 @@
         <v>3.0</v>
       </c>
       <c r="J167" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K167" s="9">
         <v>27.0</v>
@@ -6529,10 +6532,10 @@
         <v>166.0</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>18</v>
@@ -6549,7 +6552,7 @@
         <v>1.0</v>
       </c>
       <c r="J168" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K168" s="9">
         <v>27.0</v>
@@ -6560,10 +6563,10 @@
         <v>167.0</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>18</v>
@@ -6580,7 +6583,7 @@
         <v>1.0</v>
       </c>
       <c r="J169" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="K169" s="9">
         <v>27.0</v>

</xml_diff>

<commit_message>
Fix bug where 'store' cards do not advance the clock
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="378">
   <si>
     <t>type_id</t>
   </si>
@@ -4930,9 +4930,7 @@
         <v>18</v>
       </c>
       <c r="F116" s="1"/>
-      <c r="G116" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="G116" s="1"/>
       <c r="H116" s="1">
         <v>1.0</v>
       </c>
@@ -4994,9 +4992,7 @@
         <v>18</v>
       </c>
       <c r="F118" s="1"/>
-      <c r="G118" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="G118" s="1"/>
       <c r="H118" s="1">
         <v>3.0</v>
       </c>
@@ -5027,9 +5023,7 @@
         <v>18</v>
       </c>
       <c r="F119" s="1"/>
-      <c r="G119" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="G119" s="1"/>
       <c r="H119" s="1">
         <v>4.0</v>
       </c>
@@ -5060,9 +5054,7 @@
         <v>18</v>
       </c>
       <c r="F120" s="1"/>
-      <c r="G120" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="G120" s="1"/>
       <c r="H120" s="1">
         <v>5.0</v>
       </c>

</xml_diff>

<commit_message>
Add CT_SNACK (most of it)
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -576,7 +576,7 @@
     <t>Next time before you build, take 1 🃏 from the market.</t>
   </si>
   <si>
-    <t>onClient</t>
+    <t>onPreBuild</t>
   </si>
   <si>
     <t>Wind of Change</t>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="1" t="s">
+      <c r="G81" s="4" t="s">
         <v>186</v>
       </c>
       <c r="H81" s="1">
@@ -3927,8 +3927,8 @@
         <v>18</v>
       </c>
       <c r="F83" s="1"/>
-      <c r="G83" s="1" t="s">
-        <v>186</v>
+      <c r="G83" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="H83" s="1">
         <v>4.0</v>

</xml_diff>

<commit_message>
Add Mono card material
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Cards" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Mono" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="yCS/AUqO6tbZVXrRq/kgzoxiBgZysP8LVi48y8yfzAc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="iGvqM169+5TA+sSSvy1rnr3tO3ggEGKhRNRYeK4Hdy0="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="448">
   <si>
     <t>type_id</t>
   </si>
@@ -1211,12 +1212,183 @@
   <si>
     <t>While in your stall, you can include 1 junk 🃏 in each new stack.</t>
   </si>
+  <si>
+    <t>Swift Member</t>
+  </si>
+  <si>
+    <t>Mono draws 3 🃏🃏🃏. Acquire.</t>
+  </si>
+  <si>
+    <t>Loyal Member</t>
+  </si>
+  <si>
+    <t>Mono takes the highest printed valued 🃏 from the market.</t>
+  </si>
+  <si>
+    <t>Wily Member</t>
+  </si>
+  <si>
+    <t>You discard 1 random 🃏. If it is an animalfolk 🃏, Mono takes it. Acquire.</t>
+  </si>
+  <si>
+    <t>Stashing Member</t>
+  </si>
+  <si>
+    <t>Mono can use junk 🃏🃏🃏 to build this turn.</t>
+  </si>
+  <si>
+    <t>Bold Member</t>
+  </si>
+  <si>
+    <t>Roll 🐱. Swap that many 🃏🃏🃏 between the tops of your and Mono’s decks. Acquire.</t>
+  </si>
+  <si>
+    <t>Flexible Member</t>
+  </si>
+  <si>
+    <t>If Mono's discard has no Mono 🃏🃏🃏, discard Mono’s deck. Mono plays 1 Mono 🃏 from its discard.</t>
+  </si>
+  <si>
+    <t>Tireless Member</t>
+  </si>
+  <si>
+    <t>Mono swaps its lowest valued animalfolk 🃏 with the highest valued 🃏 in its stall. Acquire.</t>
+  </si>
+  <si>
+    <t>Steady Member</t>
+  </si>
+  <si>
+    <t>At the start of Mono’s next turn, it takes the leftmost 🃏 from the market.</t>
+  </si>
+  <si>
+    <t>Little Member</t>
+  </si>
+  <si>
+    <t>Mono draws 1 🃏 from your deck. It places back its lowest 🃏. Acquire.</t>
+  </si>
+  <si>
+    <t>Cunning Member</t>
+  </si>
+  <si>
+    <t>Mono draws 1 🃏 from its and your deck. It gives you the lower valued 🃏 of those. Acquire.</t>
+  </si>
+  <si>
+    <t>Daring Member</t>
+  </si>
+  <si>
+    <t>Roll 💈. Multiply the value of each 🃏 Mono uses this turn by the rolled value. Acquire.</t>
+  </si>
+  <si>
+    <t>Wise Member</t>
+  </si>
+  <si>
+    <t>If you purchased on your last turn, Mono draws 5 🃏🃏🃏. Otherwise, it draws 1 🃏. Acquire.</t>
+  </si>
+  <si>
+    <t>Master Member</t>
+  </si>
+  <si>
+    <t>Next time Mono fails to build, it takes 2 rightmost 🃏🃏 from the market and ends its action phase.</t>
+  </si>
+  <si>
+    <t>onMonoFailsToBuild</t>
+  </si>
+  <si>
+    <t>Rigorous Member</t>
+  </si>
+  <si>
+    <t>Mono discards all junk 🃏🃏🃏. It draws as many 🃏🃏🃏 +1. Acquire.</t>
+  </si>
+  <si>
+    <t>Voracious Member</t>
+  </si>
+  <si>
+    <t>Mono tosses its lowest valued animalfolk 🃏. Mono takes the highest valued 🃏 from the market.  Acquire.</t>
+  </si>
+  <si>
+    <t>Pompous Member</t>
+  </si>
+  <si>
+    <t>Discard 1 random 🃏 from your hand. If the 🃏 value matches any 🃏🃏🃏 in the market, Mono takes it. Acquire.</t>
+  </si>
+  <si>
+    <t>Carefree Member</t>
+  </si>
+  <si>
+    <t>Swap 1 animalfolk 🃏 from Mono with 1 random animalfolk 🃏 from you. Acquire.</t>
+  </si>
+  <si>
+    <t>Arcane Member</t>
+  </si>
+  <si>
+    <t>Roll 🐰. Mono draws 1 🃏 from [☄️: nowhere] [🪐: the supply] [✨: its deck]. Acquire.</t>
+  </si>
+  <si>
+    <t>Clever Member</t>
+  </si>
+  <si>
+    <t>Store the top 3 🃏🃏🃏 of Mono’s deck. Acquire.</t>
+  </si>
+  <si>
+    <t>Resourceful Member</t>
+  </si>
+  <si>
+    <t>Add +1 to Mono’s highest valued 🃏 for each junk 🃏 in its hand.</t>
+  </si>
+  <si>
+    <t>Avid Member</t>
+  </si>
+  <si>
+    <t>Mono gains 10 🟡. Acquire.</t>
+  </si>
+  <si>
+    <t>Impulsive Member</t>
+  </si>
+  <si>
+    <t>Next time Mono fails to build, it draws 3 🃏🃏🃏 and tries to build again. Acquire.</t>
+  </si>
+  <si>
+    <t>Shrewd Member</t>
+  </si>
+  <si>
+    <t>Discard 1 random 🃏. Shuffle 2 junk 🃏🃏 from your discard into your deck.</t>
+  </si>
+  <si>
+    <t>Fumbling Member</t>
+  </si>
+  <si>
+    <t>Roll ❇️ and ✳️. Look at 1 🃏 from your [source]. If it is not junk, move it into Mono's [destination]. Acquire.</t>
+  </si>
+  <si>
+    <t>Meddling Member</t>
+  </si>
+  <si>
+    <t>Place 1 junk 🃏 from Mono’s discard and 1 junk 🃏 from the junkyard on your discard. Acquire.</t>
+  </si>
+  <si>
+    <t>Dramatic Member</t>
+  </si>
+  <si>
+    <t>[🌅 Move Mono's 🕰️ 1 forward.] Mono draws [☀️ 4 🃏🃏🃏] [🌙 1 🃏].</t>
+  </si>
+  <si>
+    <t>Stealthy Member</t>
+  </si>
+  <si>
+    <t>[☀️ Move Mono's 🕰️ 1 forward.] [🌅 Mono draws 1 🃏.] [🌙 Mono takes 1 random 🃏 from you.] Acquire.</t>
+  </si>
+  <si>
+    <t>Pristine Member</t>
+  </si>
+  <si>
+    <t>Mono takes 1 junk 🃏 from the junkyard and draws 5 🃏🃏🃏. Acquire.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1240,6 +1412,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1306,7 +1483,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1365,6 +1542,57 @@
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1389,7 +1617,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="2" pivot="0" name="Sheet1-style">
+    <tableStyle count="2" pivot="0" name="Cards-style">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="1" type="secondRowStripe"/>
     </tableStyle>
@@ -1398,6 +1626,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1413,7 +1645,7 @@
     <tableColumn name="Column7" id="7"/>
     <tableColumn name="Column8" id="8"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Cards-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1631,7 +1863,8 @@
     <col customWidth="1" min="8" max="8" width="6.43"/>
     <col customWidth="1" min="9" max="9" width="10.57"/>
     <col customWidth="1" min="10" max="10" width="14.71"/>
-    <col customWidth="1" min="11" max="26" width="8.71"/>
+    <col customWidth="1" min="11" max="11" width="13.71"/>
+    <col customWidth="1" min="12" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9769,7 +10002,7 @@
       <c r="Z182" s="3"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="1"/>
+      <c r="A183" s="5"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
@@ -9797,7 +10030,7 @@
       <c r="Z183" s="3"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="1"/>
+      <c r="A184" s="5"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
@@ -32681,4 +32914,1005 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="7.71"/>
+    <col customWidth="1" min="2" max="2" width="28.71"/>
+    <col customWidth="1" min="3" max="3" width="143.29"/>
+    <col customWidth="1" min="4" max="4" width="12.86"/>
+    <col customWidth="1" min="5" max="5" width="11.29"/>
+    <col customWidth="1" min="6" max="6" width="11.0"/>
+    <col customWidth="1" min="7" max="7" width="16.0"/>
+    <col customWidth="1" min="8" max="8" width="6.43"/>
+    <col customWidth="1" min="9" max="9" width="5.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="25">
+        <f>MAX(Cards!A:A)+1</f>
+        <v>174</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I2" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="28">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="25">
+        <f t="shared" ref="A3:A29" si="1">A2+1</f>
+        <v>175</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="28">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="25">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I4" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="28">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="25">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I5" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="28">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="25">
+        <f t="shared" si="1"/>
+        <v>178</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="28">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="25">
+        <f t="shared" si="1"/>
+        <v>179</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I7" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="28">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="25">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I8" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="28">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="25">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="32">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="25">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I10" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10" s="32">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="25">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" s="32">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="25">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I12" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" s="32">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="25">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="32">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="25">
+        <f t="shared" si="1"/>
+        <v>186</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="H14" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I14" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="K14" s="32">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="25">
+        <f t="shared" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I15" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="K15" s="32">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="25">
+        <f t="shared" si="1"/>
+        <v>188</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I16" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="K16" s="32">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="25">
+        <f t="shared" si="1"/>
+        <v>189</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I17" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="32">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="25">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I18" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="K18" s="32">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="25">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I19" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="K19" s="32">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="25">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I20" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="K20" s="32">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="25">
+        <f t="shared" si="1"/>
+        <v>193</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>430</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I21" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J21" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="K21" s="32">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="25">
+        <f t="shared" si="1"/>
+        <v>194</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="H22" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I22" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J22" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="K22" s="32">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="25">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="K23" s="32">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="25">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="K24" s="32">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="25">
+        <f t="shared" si="1"/>
+        <v>197</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I25" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="K25" s="32">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="25">
+        <f t="shared" si="1"/>
+        <v>198</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>441</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I26" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="K26" s="32">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="25">
+        <f t="shared" si="1"/>
+        <v>199</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I27" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="K27" s="32">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="25">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I28" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="J28" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="K28" s="32">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="25">
+        <f t="shared" si="1"/>
+        <v>201</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I29" s="40">
+        <v>0.0</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="K29" s="28">
+        <v>28.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update deck selection portraits
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -16,8 +16,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="Q1">
+      <text>
+        <t xml:space="preserve">Not relevant for BGA. But this Sami's order
+======</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="462">
   <si>
     <t>type_id</t>
   </si>
@@ -1213,6 +1229,24 @@
     <t>While in your stall, you can include 1 junk 🃏 in each new stack.</t>
   </si>
   <si>
+    <t>animalfolk_complexity</t>
+  </si>
+  <si>
+    <t>animalfolk_interactivity</t>
+  </si>
+  <si>
+    <t>animalfolk_nastiness</t>
+  </si>
+  <si>
+    <t>animalfolk_randomness</t>
+  </si>
+  <si>
+    <t>animalfolk_game</t>
+  </si>
+  <si>
+    <t>portrait_animafolk_id</t>
+  </si>
+  <si>
     <t>Swift Member</t>
   </si>
   <si>
@@ -1382,13 +1416,37 @@
   </si>
   <si>
     <t>Mono takes 1 junk 🃏 from the junkyard and draws 5 🃏🃏🃏. Acquire.</t>
+  </si>
+  <si>
+    <t>Dodos</t>
+  </si>
+  <si>
+    <t>Capuchin Monkies</t>
+  </si>
+  <si>
+    <t>Market Manipulation</t>
+  </si>
+  <si>
+    <t>End Of Turn</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Gorilla</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1413,13 +1471,8 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1436,6 +1489,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -1483,7 +1566,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1545,20 +1628,26 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
@@ -1569,6 +1658,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1578,16 +1673,16 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -32935,6 +33030,13 @@
     <col customWidth="1" min="7" max="7" width="16.0"/>
     <col customWidth="1" min="8" max="8" width="6.43"/>
     <col customWidth="1" min="9" max="9" width="5.71"/>
+    <col customWidth="1" min="12" max="12" width="21.57"/>
+    <col customWidth="1" min="13" max="13" width="22.14"/>
+    <col customWidth="1" min="14" max="14" width="22.0"/>
+    <col customWidth="1" min="15" max="15" width="22.29"/>
+    <col customWidth="1" min="16" max="16" width="21.71"/>
+    <col customWidth="1" min="17" max="17" width="19.43"/>
+    <col customWidth="1" min="18" max="18" width="29.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -32971,25 +33073,43 @@
       <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="25">
+      <c r="A2" s="26">
         <f>MAX(Cards!A:A)+1</f>
         <v>174</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>392</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="27"/>
@@ -32999,25 +33119,43 @@
       <c r="I2" s="28">
         <v>0.0</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="27" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="28">
         <v>1.0</v>
       </c>
+      <c r="L2" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M2" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N2" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O2" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P2" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q2" s="21">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="25">
-        <f t="shared" ref="A3:A29" si="1">A2+1</f>
+      <c r="A3" s="26">
+        <f t="shared" ref="A3:A37" si="1">A2+1</f>
         <v>175</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="B3" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="27"/>
@@ -33029,31 +33167,49 @@
       <c r="I3" s="28">
         <v>0.0</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="27" t="s">
         <v>33</v>
       </c>
       <c r="K3" s="28">
         <v>2.0</v>
       </c>
+      <c r="L3" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="N3" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O3" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P3" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="25">
+      <c r="A4" s="26">
         <f t="shared" si="1"/>
         <v>176</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>396</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>402</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="27"/>
@@ -33063,28 +33219,46 @@
       <c r="I4" s="28">
         <v>0.0</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="27" t="s">
         <v>46</v>
       </c>
       <c r="K4" s="28">
         <v>3.0</v>
       </c>
+      <c r="L4" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M4" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N4" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O4" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P4" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="25">
+      <c r="A5" s="26">
         <f t="shared" si="1"/>
         <v>177</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>397</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>398</v>
-      </c>
-      <c r="D5" s="26" t="s">
+      <c r="B5" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>404</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="27" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="27"/>
@@ -33095,31 +33269,49 @@
       <c r="I5" s="28">
         <v>0.0</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="27" t="s">
         <v>59</v>
       </c>
       <c r="K5" s="28">
         <v>4.0</v>
       </c>
+      <c r="L5" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P5" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="25">
+      <c r="A6" s="26">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>399</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>400</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>406</v>
+      </c>
+      <c r="D6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="27"/>
@@ -33129,28 +33321,46 @@
       <c r="I6" s="28">
         <v>0.0</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="27" t="s">
         <v>72</v>
       </c>
       <c r="K6" s="28">
         <v>5.0</v>
       </c>
+      <c r="L6" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M6" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N6" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="O6" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="P6" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="25">
+      <c r="A7" s="26">
         <f t="shared" si="1"/>
         <v>179</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>401</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>402</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="27"/>
@@ -33161,31 +33371,49 @@
       <c r="I7" s="28">
         <v>0.0</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="27" t="s">
         <v>85</v>
       </c>
       <c r="K7" s="28">
         <v>6.0</v>
       </c>
+      <c r="L7" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M7" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P7" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="25">
+      <c r="A8" s="26">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>404</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="27"/>
@@ -33195,32 +33423,50 @@
       <c r="I8" s="28">
         <v>0.0</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="27" t="s">
         <v>98</v>
       </c>
       <c r="K8" s="28">
         <v>7.0</v>
       </c>
+      <c r="L8" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M8" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P8" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="25">
+      <c r="A9" s="26">
         <f t="shared" si="1"/>
         <v>181</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>406</v>
-      </c>
-      <c r="D9" s="26" t="s">
+      <c r="B9" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="27"/>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="27" t="s">
         <v>111</v>
       </c>
       <c r="H9" s="28">
@@ -33229,31 +33475,49 @@
       <c r="I9" s="28">
         <v>0.0</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="34">
         <v>8.0</v>
       </c>
+      <c r="L9" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M9" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O9" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P9" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="25">
+      <c r="A10" s="26">
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>407</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>408</v>
-      </c>
-      <c r="D10" s="26" t="s">
+      <c r="B10" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="27"/>
@@ -33263,31 +33527,49 @@
       <c r="I10" s="28">
         <v>0.0</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="34">
         <v>9.0</v>
       </c>
+      <c r="L10" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M10" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N10" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O10" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P10" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="25">
+      <c r="A11" s="26">
         <f t="shared" si="1"/>
         <v>183</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>409</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>410</v>
-      </c>
-      <c r="D11" s="26" t="s">
+      <c r="B11" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>416</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="27"/>
@@ -33297,31 +33579,49 @@
       <c r="I11" s="28">
         <v>0.0</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="34">
         <v>10.0</v>
       </c>
+      <c r="L11" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M11" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N11" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="O11" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P11" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="25">
+      <c r="A12" s="26">
         <f t="shared" si="1"/>
         <v>184</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>411</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>412</v>
-      </c>
-      <c r="D12" s="26" t="s">
+      <c r="B12" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="27"/>
@@ -33331,31 +33631,49 @@
       <c r="I12" s="28">
         <v>0.0</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="34">
         <v>11.0</v>
       </c>
+      <c r="L12" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M12" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O12" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="P12" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="25">
+      <c r="A13" s="26">
         <f t="shared" si="1"/>
         <v>185</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>413</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="D13" s="26" t="s">
+      <c r="B13" s="30" t="s">
+        <v>419</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>420</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="27"/>
@@ -33365,31 +33683,49 @@
       <c r="I13" s="28">
         <v>0.0</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="34">
         <v>12.0</v>
       </c>
+      <c r="L13" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M13" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O13" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P13" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="25">
+      <c r="A14" s="26">
         <f t="shared" si="1"/>
         <v>186</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>416</v>
-      </c>
-      <c r="D14" s="26" t="s">
+      <c r="B14" s="27" t="s">
+        <v>421</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
-      <c r="G14" s="26" t="s">
-        <v>417</v>
+      <c r="G14" s="27" t="s">
+        <v>423</v>
       </c>
       <c r="H14" s="28">
         <v>2.0</v>
@@ -33397,31 +33733,49 @@
       <c r="I14" s="28">
         <v>0.0</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="34">
         <v>13.0</v>
       </c>
+      <c r="L14" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M14" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O14" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P14" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="25">
+      <c r="A15" s="26">
         <f t="shared" si="1"/>
         <v>187</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="D15" s="26" t="s">
+      <c r="B15" s="27" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>425</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="27"/>
@@ -33431,31 +33785,49 @@
       <c r="I15" s="28">
         <v>0.0</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="34">
         <v>14.0</v>
       </c>
+      <c r="L15" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M15" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N15" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P15" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="25">
+      <c r="A16" s="26">
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>421</v>
-      </c>
-      <c r="D16" s="26" t="s">
+      <c r="B16" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>427</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="27"/>
@@ -33465,31 +33837,49 @@
       <c r="I16" s="28">
         <v>0.0</v>
       </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="34">
         <v>15.0</v>
       </c>
+      <c r="L16" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M16" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P16" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="25">
+      <c r="A17" s="26">
         <f t="shared" si="1"/>
         <v>189</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="D17" s="26" t="s">
+      <c r="B17" s="27" t="s">
+        <v>428</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="27"/>
@@ -33499,31 +33889,49 @@
       <c r="I17" s="28">
         <v>0.0</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="34">
         <v>16.0</v>
       </c>
+      <c r="L17" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M17" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N17" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O17" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P17" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="25">
+      <c r="A18" s="26">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>424</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>425</v>
-      </c>
-      <c r="D18" s="26" t="s">
+      <c r="B18" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="D18" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="27"/>
@@ -33533,31 +33941,49 @@
       <c r="I18" s="28">
         <v>0.0</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="34">
         <v>17.0</v>
       </c>
+      <c r="L18" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M18" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N18" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="O18" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P18" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="25">
+      <c r="A19" s="26">
         <f t="shared" si="1"/>
         <v>191</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>427</v>
-      </c>
-      <c r="D19" s="26" t="s">
+      <c r="B19" s="27" t="s">
+        <v>432</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>433</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="27"/>
@@ -33567,352 +33993,887 @@
       <c r="I19" s="28">
         <v>0.0</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="K19" s="32">
+      <c r="K19" s="34">
         <v>18.0</v>
       </c>
+      <c r="L19" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M19" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N19" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O19" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="P19" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="25">
+      <c r="A20" s="26">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>428</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>429</v>
-      </c>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="27" t="s">
+        <v>434</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>435</v>
+      </c>
+      <c r="D20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="27" t="s">
         <v>111</v>
       </c>
       <c r="H20" s="28">
         <v>2.0</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="38">
         <v>0.0</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="K20" s="32">
+      <c r="K20" s="34">
         <v>19.0</v>
       </c>
+      <c r="L20" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M20" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O20" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P20" s="36">
+        <v>3.0</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>18.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="25">
+      <c r="A21" s="26">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="D21" s="26" t="s">
+      <c r="B21" s="27" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>437</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="28">
         <v>2.0</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="38">
         <v>0.0</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="K21" s="32">
+      <c r="K21" s="34">
         <v>20.0</v>
       </c>
+      <c r="L21" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M21" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N21" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O21" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P21" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="25">
+      <c r="A22" s="26">
         <f t="shared" si="1"/>
         <v>194</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>433</v>
-      </c>
-      <c r="D22" s="26" t="s">
+      <c r="B22" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>439</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="26" t="s">
-        <v>417</v>
+      <c r="G22" s="27" t="s">
+        <v>423</v>
       </c>
       <c r="H22" s="28">
         <v>2.0</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="38">
         <v>0.0</v>
       </c>
-      <c r="J22" s="35" t="s">
+      <c r="J22" s="39" t="s">
         <v>288</v>
       </c>
-      <c r="K22" s="32">
+      <c r="K22" s="34">
         <v>21.0</v>
       </c>
+      <c r="L22" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M22" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N22" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O22" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P22" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="25">
+      <c r="A23" s="26">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>434</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="D23" s="26" t="s">
+      <c r="B23" s="27" t="s">
+        <v>440</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="37"/>
       <c r="H23" s="28">
         <v>2.0</v>
       </c>
-      <c r="I23" s="34">
+      <c r="I23" s="38">
         <v>0.0</v>
       </c>
-      <c r="J23" s="35" t="s">
+      <c r="J23" s="39" t="s">
         <v>302</v>
       </c>
-      <c r="K23" s="32">
+      <c r="K23" s="34">
         <v>22.0</v>
       </c>
+      <c r="L23" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M23" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N23" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O23" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P23" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="25">
+      <c r="A24" s="26">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>437</v>
-      </c>
-      <c r="D24" s="26" t="s">
+      <c r="B24" s="27" t="s">
+        <v>442</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>443</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="28">
         <v>2.0</v>
       </c>
-      <c r="I24" s="34">
+      <c r="I24" s="38">
         <v>0.0</v>
       </c>
-      <c r="J24" s="35" t="s">
+      <c r="J24" s="39" t="s">
         <v>315</v>
       </c>
-      <c r="K24" s="32">
+      <c r="K24" s="34">
         <v>23.0</v>
       </c>
+      <c r="L24" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M24" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N24" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="O24" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P24" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="25">
+      <c r="A25" s="26">
         <f t="shared" si="1"/>
         <v>197</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>438</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>439</v>
-      </c>
-      <c r="D25" s="26" t="s">
+      <c r="B25" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>445</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="36"/>
+      <c r="G25" s="37"/>
       <c r="H25" s="28">
         <v>2.0</v>
       </c>
-      <c r="I25" s="34">
+      <c r="I25" s="38">
         <v>0.0</v>
       </c>
-      <c r="J25" s="35" t="s">
+      <c r="J25" s="39" t="s">
         <v>328</v>
       </c>
-      <c r="K25" s="32">
+      <c r="K25" s="34">
         <v>24.0</v>
       </c>
+      <c r="L25" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M25" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N25" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O25" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="P25" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>25.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="25">
+      <c r="A26" s="26">
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>441</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="B26" s="43" t="s">
+        <v>446</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="D26" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="36"/>
+      <c r="G26" s="37"/>
       <c r="H26" s="28">
         <v>2.0</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="38">
         <v>0.0</v>
       </c>
-      <c r="J26" s="35" t="s">
+      <c r="J26" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="K26" s="32">
+      <c r="K26" s="34">
         <v>25.0</v>
       </c>
+      <c r="L26" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M26" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="N26" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="O26" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P26" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="25">
+      <c r="A27" s="26">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>442</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>443</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="B27" s="27" t="s">
+        <v>448</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>449</v>
+      </c>
+      <c r="D27" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
       <c r="H27" s="28">
         <v>2.0</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="38">
         <v>0.0</v>
       </c>
-      <c r="J27" s="35" t="s">
+      <c r="J27" s="39" t="s">
         <v>354</v>
       </c>
-      <c r="K27" s="32">
+      <c r="K27" s="34">
         <v>26.0</v>
       </c>
+      <c r="L27" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M27" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N27" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O27" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P27" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>27.0</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="25">
+      <c r="A28" s="26">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>444</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>445</v>
-      </c>
-      <c r="D28" s="26" t="s">
+      <c r="B28" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>451</v>
+      </c>
+      <c r="D28" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="37"/>
       <c r="H28" s="28">
         <v>2.0</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28" s="38">
         <v>0.0</v>
       </c>
-      <c r="J28" s="35" t="s">
+      <c r="J28" s="39" t="s">
         <v>367</v>
       </c>
-      <c r="K28" s="32">
+      <c r="K28" s="34">
         <v>27.0</v>
       </c>
+      <c r="L28" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M28" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N28" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O28" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P28" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>28.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="25">
+      <c r="A29" s="26">
         <f t="shared" si="1"/>
         <v>201</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>446</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="D29" s="26" t="s">
+      <c r="B29" s="27" t="s">
+        <v>452</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="D29" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="38" t="s">
+      <c r="F29" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="39"/>
+      <c r="G29" s="43"/>
       <c r="H29" s="28">
         <v>2.0</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="44">
         <v>0.0</v>
       </c>
-      <c r="J29" s="33" t="s">
+      <c r="J29" s="37" t="s">
         <v>380</v>
       </c>
       <c r="K29" s="28">
         <v>28.0</v>
       </c>
+      <c r="L29" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M29" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N29" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O29" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P29" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q29" s="21">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="26">
+        <f t="shared" si="1"/>
+        <v>202</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I30" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="K30" s="34">
+        <v>29.0</v>
+      </c>
+      <c r="L30" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M30" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N30" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O30" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P30" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q30" s="21">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="26">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I31" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="K31" s="28">
+        <v>30.0</v>
+      </c>
+      <c r="L31" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M31" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N31" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="O31" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P31" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q31" s="21">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="26">
+        <f t="shared" si="1"/>
+        <v>204</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I32" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="K32" s="34">
+        <v>31.0</v>
+      </c>
+      <c r="L32" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M32" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="N32" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="O32" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="P32" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="26">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I33" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="K33" s="34">
+        <v>32.0</v>
+      </c>
+      <c r="L33" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M33" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N33" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O33" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P33" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="26">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I34" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="K34" s="28">
+        <v>33.0</v>
+      </c>
+      <c r="L34" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="M34" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N34" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O34" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P34" s="35">
+        <v>5.0</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="26">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I35" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="K35" s="34">
+        <v>34.0</v>
+      </c>
+      <c r="L35" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="M35" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N35" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O35" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P35" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="26">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I36" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="K36" s="34">
+        <v>35.0</v>
+      </c>
+      <c r="L36" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="M36" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="N36" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O36" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="P36" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q36" s="21">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="26">
+        <f t="shared" si="1"/>
+        <v>209</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="I37" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="K37" s="28">
+        <v>36.0</v>
+      </c>
+      <c r="L37" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="M37" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="N37" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="O37" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P37" s="42">
+        <v>6.0</v>
+      </c>
+      <c r="Q37" s="21">
+        <v>36.0</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reduce margins to fit 8 animalfolk portraits in 1 row
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -33801,7 +33801,7 @@
         <v>0.0</v>
       </c>
       <c r="O15" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" s="36">
         <v>3.0</v>
@@ -34854,16 +34854,16 @@
         <v>36.0</v>
       </c>
       <c r="L37" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M37" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N37" s="21">
         <v>0.0</v>
       </c>
       <c r="O37" s="21">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P37" s="42">
         <v>6.0</v>

</xml_diff>

<commit_message>
Update syling based on Sami's feedback
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_10thanniversary.xlsx
+++ b/misc/genmaterial/material_10thanniversary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="462">
   <si>
     <t>type_id</t>
   </si>
@@ -1566,7 +1566,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1660,6 +1660,9 @@
     </xf>
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -33462,9 +33465,7 @@
       <c r="D9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>18</v>
-      </c>
+      <c r="E9" s="27"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27" t="s">
         <v>111</v>
@@ -33800,10 +33801,10 @@
       <c r="N15" s="21">
         <v>0.0</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="36">
         <v>1.0</v>
       </c>
-      <c r="P15" s="36">
+      <c r="P15" s="37">
         <v>3.0</v>
       </c>
       <c r="Q15" s="21">
@@ -33855,7 +33856,7 @@
       <c r="O16" s="21">
         <v>2.0</v>
       </c>
-      <c r="P16" s="36">
+      <c r="P16" s="37">
         <v>3.0</v>
       </c>
       <c r="Q16" s="21">
@@ -33907,7 +33908,7 @@
       <c r="O17" s="21">
         <v>2.0</v>
       </c>
-      <c r="P17" s="36">
+      <c r="P17" s="37">
         <v>3.0</v>
       </c>
       <c r="Q17" s="21">
@@ -33959,7 +33960,7 @@
       <c r="O18" s="21">
         <v>2.0</v>
       </c>
-      <c r="P18" s="36">
+      <c r="P18" s="37">
         <v>3.0</v>
       </c>
       <c r="Q18" s="21">
@@ -34011,7 +34012,7 @@
       <c r="O19" s="21">
         <v>3.0</v>
       </c>
-      <c r="P19" s="36">
+      <c r="P19" s="37">
         <v>3.0</v>
       </c>
       <c r="Q19" s="21">
@@ -34035,7 +34036,7 @@
       <c r="E20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="38" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="27" t="s">
@@ -34044,10 +34045,10 @@
       <c r="H20" s="28">
         <v>2.0</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="39">
         <v>0.0</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="40" t="s">
         <v>262</v>
       </c>
       <c r="K20" s="34">
@@ -34065,7 +34066,7 @@
       <c r="O20" s="21">
         <v>1.0</v>
       </c>
-      <c r="P20" s="36">
+      <c r="P20" s="37">
         <v>3.0</v>
       </c>
       <c r="Q20" s="21">
@@ -34089,15 +34090,15 @@
       <c r="E21" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="28">
         <v>2.0</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="39">
         <v>0.0</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="40" t="s">
         <v>275</v>
       </c>
       <c r="K21" s="34">
@@ -34115,7 +34116,7 @@
       <c r="O21" s="21">
         <v>1.0</v>
       </c>
-      <c r="P21" s="40">
+      <c r="P21" s="41">
         <v>4.0</v>
       </c>
       <c r="Q21" s="21">
@@ -34130,7 +34131,7 @@
       <c r="B22" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="42" t="s">
         <v>439</v>
       </c>
       <c r="D22" s="27" t="s">
@@ -34139,7 +34140,7 @@
       <c r="E22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="38" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="27" t="s">
@@ -34148,10 +34149,10 @@
       <c r="H22" s="28">
         <v>2.0</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="39">
         <v>0.0</v>
       </c>
-      <c r="J22" s="39" t="s">
+      <c r="J22" s="40" t="s">
         <v>288</v>
       </c>
       <c r="K22" s="34">
@@ -34169,7 +34170,7 @@
       <c r="O22" s="21">
         <v>1.0</v>
       </c>
-      <c r="P22" s="40">
+      <c r="P22" s="41">
         <v>4.0</v>
       </c>
       <c r="Q22" s="21">
@@ -34193,17 +34194,17 @@
       <c r="E23" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="37"/>
+      <c r="G23" s="38"/>
       <c r="H23" s="28">
         <v>2.0</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="39">
         <v>0.0</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="40" t="s">
         <v>302</v>
       </c>
       <c r="K23" s="34">
@@ -34221,7 +34222,7 @@
       <c r="O23" s="21">
         <v>1.0</v>
       </c>
-      <c r="P23" s="40">
+      <c r="P23" s="41">
         <v>4.0</v>
       </c>
       <c r="Q23" s="21">
@@ -34245,15 +34246,15 @@
       <c r="E24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
       <c r="H24" s="28">
         <v>2.0</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="39">
         <v>0.0</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="40" t="s">
         <v>315</v>
       </c>
       <c r="K24" s="34">
@@ -34271,7 +34272,7 @@
       <c r="O24" s="21">
         <v>2.0</v>
       </c>
-      <c r="P24" s="42">
+      <c r="P24" s="43">
         <v>6.0</v>
       </c>
       <c r="Q24" s="21">
@@ -34295,17 +34296,17 @@
       <c r="E25" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="37"/>
+      <c r="G25" s="38"/>
       <c r="H25" s="28">
         <v>2.0</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="39">
         <v>0.0</v>
       </c>
-      <c r="J25" s="39" t="s">
+      <c r="J25" s="40" t="s">
         <v>328</v>
       </c>
       <c r="K25" s="34">
@@ -34335,10 +34336,10 @@
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="44" t="s">
         <v>446</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="42" t="s">
         <v>447</v>
       </c>
       <c r="D26" s="27" t="s">
@@ -34347,17 +34348,17 @@
       <c r="E26" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="37"/>
+      <c r="G26" s="38"/>
       <c r="H26" s="28">
         <v>2.0</v>
       </c>
-      <c r="I26" s="38">
+      <c r="I26" s="39">
         <v>0.0</v>
       </c>
-      <c r="J26" s="39" t="s">
+      <c r="J26" s="40" t="s">
         <v>341</v>
       </c>
       <c r="K26" s="34">
@@ -34399,15 +34400,15 @@
       <c r="E27" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
       <c r="H27" s="28">
         <v>2.0</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="39">
         <v>0.0</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="40" t="s">
         <v>354</v>
       </c>
       <c r="K27" s="34">
@@ -34425,7 +34426,7 @@
       <c r="O27" s="21">
         <v>1.0</v>
       </c>
-      <c r="P27" s="42">
+      <c r="P27" s="43">
         <v>6.0</v>
       </c>
       <c r="Q27" s="21">
@@ -34449,17 +34450,17 @@
       <c r="E28" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="37"/>
+      <c r="G28" s="38"/>
       <c r="H28" s="28">
         <v>2.0</v>
       </c>
-      <c r="I28" s="38">
+      <c r="I28" s="39">
         <v>0.0</v>
       </c>
-      <c r="J28" s="39" t="s">
+      <c r="J28" s="40" t="s">
         <v>367</v>
       </c>
       <c r="K28" s="34">
@@ -34477,7 +34478,7 @@
       <c r="O28" s="21">
         <v>2.0</v>
       </c>
-      <c r="P28" s="42">
+      <c r="P28" s="43">
         <v>6.0</v>
       </c>
       <c r="Q28" s="21">
@@ -34501,17 +34502,17 @@
       <c r="E29" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="43"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="28">
         <v>2.0</v>
       </c>
-      <c r="I29" s="44">
+      <c r="I29" s="45">
         <v>0.0</v>
       </c>
-      <c r="J29" s="37" t="s">
+      <c r="J29" s="38" t="s">
         <v>380</v>
       </c>
       <c r="K29" s="28">
@@ -34550,7 +34551,7 @@
       <c r="H30" s="28">
         <v>2.0</v>
       </c>
-      <c r="I30" s="44">
+      <c r="I30" s="45">
         <v>0.0</v>
       </c>
       <c r="J30" s="21" t="s">
@@ -34571,7 +34572,7 @@
       <c r="O30" s="21">
         <v>1.0</v>
       </c>
-      <c r="P30" s="40">
+      <c r="P30" s="41">
         <v>4.0</v>
       </c>
       <c r="Q30" s="21">
@@ -34592,7 +34593,7 @@
       <c r="H31" s="28">
         <v>2.0</v>
       </c>
-      <c r="I31" s="44">
+      <c r="I31" s="45">
         <v>0.0</v>
       </c>
       <c r="J31" s="21" t="s">
@@ -34613,7 +34614,7 @@
       <c r="O31" s="21">
         <v>1.0</v>
       </c>
-      <c r="P31" s="40">
+      <c r="P31" s="41">
         <v>4.0</v>
       </c>
       <c r="Q31" s="21">
@@ -34634,7 +34635,7 @@
       <c r="H32" s="28">
         <v>2.0</v>
       </c>
-      <c r="I32" s="44">
+      <c r="I32" s="45">
         <v>0.0</v>
       </c>
       <c r="J32" s="21" t="s">
@@ -34655,7 +34656,7 @@
       <c r="O32" s="21">
         <v>2.0</v>
       </c>
-      <c r="P32" s="40">
+      <c r="P32" s="41">
         <v>4.0</v>
       </c>
       <c r="Q32" s="21">
@@ -34676,7 +34677,7 @@
       <c r="H33" s="28">
         <v>2.0</v>
       </c>
-      <c r="I33" s="44">
+      <c r="I33" s="45">
         <v>0.0</v>
       </c>
       <c r="J33" s="21" t="s">
@@ -34718,7 +34719,7 @@
       <c r="H34" s="28">
         <v>2.0</v>
       </c>
-      <c r="I34" s="44">
+      <c r="I34" s="45">
         <v>0.0</v>
       </c>
       <c r="J34" s="21" t="s">
@@ -34760,7 +34761,7 @@
       <c r="H35" s="28">
         <v>2.0</v>
       </c>
-      <c r="I35" s="44">
+      <c r="I35" s="45">
         <v>0.0</v>
       </c>
       <c r="J35" s="21" t="s">
@@ -34781,7 +34782,7 @@
       <c r="O35" s="21">
         <v>1.0</v>
       </c>
-      <c r="P35" s="42">
+      <c r="P35" s="43">
         <v>6.0</v>
       </c>
       <c r="Q35" s="21">
@@ -34802,7 +34803,7 @@
       <c r="H36" s="28">
         <v>2.0</v>
       </c>
-      <c r="I36" s="44">
+      <c r="I36" s="45">
         <v>0.0</v>
       </c>
       <c r="J36" s="21" t="s">
@@ -34823,7 +34824,7 @@
       <c r="O36" s="21">
         <v>1.0</v>
       </c>
-      <c r="P36" s="42">
+      <c r="P36" s="43">
         <v>6.0</v>
       </c>
       <c r="Q36" s="21">
@@ -34844,7 +34845,7 @@
       <c r="H37" s="28">
         <v>2.0</v>
       </c>
-      <c r="I37" s="44">
+      <c r="I37" s="45">
         <v>0.0</v>
       </c>
       <c r="J37" s="21" t="s">
@@ -34865,7 +34866,7 @@
       <c r="O37" s="21">
         <v>1.0</v>
       </c>
-      <c r="P37" s="42">
+      <c r="P37" s="43">
         <v>6.0</v>
       </c>
       <c r="Q37" s="21">

</xml_diff>